<commit_message>
New version of assembly list
</commit_message>
<xml_diff>
--- a/Dissertation_Assembly_list.xlsx
+++ b/Dissertation_Assembly_list.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frankieswift/Desktop/Dissertation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frankieswift/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4CE5DA81-87DA-034E-91D4-F1947AEFC811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F6CBB50F-AC7A-114B-8D40-252A210723BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" xr2:uid="{B0177056-D2ED-5444-891D-4508833FC62F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="343">
   <si>
     <t xml:space="preserve">name </t>
   </si>
@@ -723,21 +723,6 @@
   </si>
   <si>
     <t>GCA_905147745.1</t>
-  </si>
-  <si>
-    <t>Omphaloscelis lunosa (moths)</t>
-  </si>
-  <si>
-    <t>ilOmpLuno1.1</t>
-  </si>
-  <si>
-    <t>GCA_916610225.1</t>
-  </si>
-  <si>
-    <t>GCA_916610215.1</t>
-  </si>
-  <si>
-    <t>assembly broken fixing it</t>
   </si>
   <si>
     <t>Xestia xanthographa (moths)</t>
@@ -1546,10 +1531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E3F9800-BE78-5B4C-8975-4378731B835F}">
-  <dimension ref="A1:K101"/>
+  <dimension ref="A1:K100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55:XFD55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1570,25 +1555,25 @@
   <sheetData>
     <row r="1" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>2</v>
@@ -3314,7 +3299,7 @@
         <v>507279681</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="10" t="s">
         <v>229</v>
       </c>
@@ -3330,685 +3315,687 @@
       <c r="E57" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F57" s="2"/>
-      <c r="G57" s="1" t="s">
-        <v>233</v>
+      <c r="F57" s="2">
+        <v>98.7</v>
+      </c>
+      <c r="G57" s="2">
+        <v>1.2607439581338401E-2</v>
       </c>
       <c r="H57" s="1">
-        <v>1.2800000000000001E-2</v>
+        <v>2.0899999999999998E-2</v>
       </c>
       <c r="I57" s="11"/>
       <c r="J57" s="12">
-        <v>661871610</v>
+        <v>933835876</v>
       </c>
       <c r="K57" s="12">
-        <v>623261760</v>
+        <v>878409741</v>
       </c>
     </row>
     <row r="58" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="B58" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="C58" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="D58" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="D58" s="1" t="s">
-        <v>237</v>
-      </c>
       <c r="E58" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F58" s="2">
-        <v>98.7</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="F58" s="2"/>
       <c r="G58" s="2">
-        <v>1.2607439581338401E-2</v>
-      </c>
-      <c r="H58" s="1">
-        <v>2.0899999999999998E-2</v>
-      </c>
-      <c r="I58" s="11"/>
+        <v>9.0490235598815298E-3</v>
+      </c>
+      <c r="I58" s="17"/>
       <c r="J58" s="12">
-        <v>933835876</v>
+        <v>399722661</v>
       </c>
       <c r="K58" s="12">
-        <v>878409741</v>
+        <v>375808107</v>
       </c>
     </row>
     <row r="59" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="B59" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="C59" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="D59" s="1" t="s">
         <v>240</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>241</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F59" s="2"/>
       <c r="G59" s="2">
-        <v>9.0490235598815298E-3</v>
+        <v>1.7970123165282199E-2</v>
       </c>
       <c r="I59" s="17"/>
       <c r="J59" s="12">
-        <v>399722661</v>
+        <v>276688267</v>
       </c>
       <c r="K59" s="12">
-        <v>375808107</v>
+        <v>259778591</v>
       </c>
     </row>
     <row r="60" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="B60" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="B60" s="3" t="s">
+      <c r="C60" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="D60" s="1" t="s">
         <v>244</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>245</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F60" s="2"/>
       <c r="G60" s="2">
-        <v>1.7970123165282199E-2</v>
-      </c>
-      <c r="I60" s="17"/>
+        <v>1.31357182632922E-2</v>
+      </c>
+      <c r="H60" s="1">
+        <v>1.4800000000000001E-2</v>
+      </c>
+      <c r="I60" s="11"/>
       <c r="J60" s="12">
-        <v>276688267</v>
+        <v>430396360</v>
       </c>
       <c r="K60" s="12">
-        <v>259778591</v>
+        <v>404075388</v>
       </c>
     </row>
     <row r="61" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="B61" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="B61" s="3" t="s">
+      <c r="C61" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="D61" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="D61" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F61" s="2"/>
+      <c r="E61" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="G61" s="2">
-        <v>1.31357182632922E-2</v>
+        <v>1.8630198584859099E-2</v>
       </c>
       <c r="H61" s="1">
-        <v>1.4800000000000001E-2</v>
-      </c>
-      <c r="I61" s="11"/>
+        <v>1.9599999999999999E-2</v>
+      </c>
+      <c r="I61" s="14"/>
       <c r="J61" s="12">
-        <v>430396360</v>
+        <v>709796853</v>
       </c>
       <c r="K61" s="12">
-        <v>404075388</v>
+        <v>664534381</v>
       </c>
     </row>
     <row r="62" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="B62" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="B62" s="3" t="s">
+      <c r="C62" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="C62" s="1" t="s">
+      <c r="D62" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="D62" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="E62" s="1" t="s">
+      <c r="E62" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="F62" s="2"/>
       <c r="G62" s="2">
-        <v>1.8630198584859099E-2</v>
-      </c>
-      <c r="H62" s="1">
-        <v>1.9599999999999999E-2</v>
-      </c>
-      <c r="I62" s="14"/>
+        <v>8.7960966728474702E-3</v>
+      </c>
+      <c r="I62" s="11"/>
       <c r="J62" s="12">
-        <v>709796853</v>
+        <v>978296047</v>
       </c>
       <c r="K62" s="12">
-        <v>664534381</v>
+        <v>915863888</v>
       </c>
     </row>
     <row r="63" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="10" t="s">
+        <v>253</v>
+      </c>
+      <c r="B63" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="C63" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="D63" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="D63" s="1" t="s">
-        <v>257</v>
-      </c>
       <c r="E63" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F63" s="2"/>
+        <v>28</v>
+      </c>
+      <c r="F63" s="2">
+        <v>99.1</v>
+      </c>
       <c r="G63" s="2">
-        <v>8.7960966728474702E-3</v>
+        <v>1.11266721490465E-2</v>
+      </c>
+      <c r="H63" s="1">
+        <v>1.2E-2</v>
       </c>
       <c r="I63" s="11"/>
       <c r="J63" s="12">
-        <v>978296047</v>
+        <v>370417233</v>
       </c>
       <c r="K63" s="12">
-        <v>915863888</v>
+        <v>345513544</v>
       </c>
     </row>
     <row r="64" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="B64" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="C64" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="D64" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="D64" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="E64" s="2" t="s">
+      <c r="E64" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F64" s="2">
-        <v>99.1</v>
+      <c r="F64" s="1">
+        <v>98.9</v>
       </c>
       <c r="G64" s="2">
-        <v>1.11266721490465E-2</v>
+        <v>1.25732129149967E-2</v>
       </c>
       <c r="H64" s="1">
-        <v>1.2E-2</v>
-      </c>
-      <c r="I64" s="11"/>
+        <v>1.3999999999999999E-2</v>
+      </c>
+      <c r="I64" s="14"/>
       <c r="J64" s="12">
-        <v>370417233</v>
+        <v>484822887</v>
       </c>
       <c r="K64" s="12">
-        <v>345513544</v>
+        <v>452203855</v>
       </c>
     </row>
     <row r="65" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" s="10" t="s">
+        <v>261</v>
+      </c>
+      <c r="B65" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="B65" s="3" t="s">
+      <c r="C65" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="C65" s="1" t="s">
+      <c r="D65" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="D65" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="E65" s="1" t="s">
+      <c r="E65" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F65" s="1">
-        <v>98.9</v>
+      <c r="F65" s="2">
+        <v>98.3</v>
       </c>
       <c r="G65" s="2">
-        <v>1.25732129149967E-2</v>
+        <v>2.2160365458540401E-2</v>
       </c>
       <c r="H65" s="1">
-        <v>1.3999999999999999E-2</v>
-      </c>
-      <c r="I65" s="14"/>
+        <v>2.4399999999999998E-2</v>
+      </c>
+      <c r="I65" s="11"/>
       <c r="J65" s="12">
-        <v>484822887</v>
+        <v>402035149</v>
       </c>
       <c r="K65" s="12">
-        <v>452203855</v>
+        <v>374714401</v>
       </c>
     </row>
     <row r="66" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="10" t="s">
+        <v>265</v>
+      </c>
+      <c r="B66" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="B66" s="3" t="s">
+      <c r="C66" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="C66" s="1" t="s">
+      <c r="D66" s="1" t="s">
         <v>268</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>269</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F66" s="2">
-        <v>98.3</v>
-      </c>
+      <c r="F66" s="2"/>
       <c r="G66" s="2">
-        <v>2.2160365458540401E-2</v>
-      </c>
-      <c r="H66" s="1">
-        <v>2.4399999999999998E-2</v>
-      </c>
-      <c r="I66" s="11"/>
+        <v>2.6042409117566102E-2</v>
+      </c>
+      <c r="I66" s="17"/>
       <c r="J66" s="12">
-        <v>402035149</v>
+        <v>403420000</v>
       </c>
       <c r="K66" s="12">
-        <v>374714401</v>
+        <v>374514753</v>
       </c>
     </row>
     <row r="67" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="10" t="s">
+        <v>269</v>
+      </c>
+      <c r="B67" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="B67" s="3" t="s">
+      <c r="C67" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="C67" s="1" t="s">
+      <c r="D67" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="D67" s="1" t="s">
-        <v>273</v>
-      </c>
       <c r="E67" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F67" s="2"/>
+        <v>23</v>
+      </c>
+      <c r="F67" s="2">
+        <v>98.1</v>
+      </c>
       <c r="G67" s="2">
-        <v>2.6042409117566102E-2</v>
-      </c>
-      <c r="I67" s="17"/>
+        <v>1.97678842325568E-2</v>
+      </c>
+      <c r="H67" s="1">
+        <v>2.4900000000000002E-2</v>
+      </c>
+      <c r="I67" s="11"/>
       <c r="J67" s="12">
-        <v>403420000</v>
+        <v>462005964</v>
       </c>
       <c r="K67" s="12">
-        <v>374514753</v>
+        <v>428788595</v>
       </c>
     </row>
     <row r="68" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="B68" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="B68" s="3" t="s">
+      <c r="C68" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="C68" s="1" t="s">
+      <c r="D68" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="D68" s="1" t="s">
-        <v>277</v>
-      </c>
       <c r="E68" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F68" s="2">
-        <v>98.1</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="F68" s="2"/>
       <c r="G68" s="2">
-        <v>1.97678842325568E-2</v>
+        <v>6.9371728010743103E-3</v>
       </c>
       <c r="H68" s="1">
-        <v>2.4900000000000002E-2</v>
-      </c>
-      <c r="I68" s="11"/>
+        <v>1.34E-2</v>
+      </c>
+      <c r="I68" s="17"/>
       <c r="J68" s="12">
-        <v>462005964</v>
+        <v>1334036499</v>
       </c>
       <c r="K68" s="12">
-        <v>428788595</v>
+        <v>1237756284</v>
       </c>
     </row>
     <row r="69" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="B69" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="B69" s="3" t="s">
+      <c r="C69" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="C69" s="1" t="s">
+      <c r="D69" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="D69" s="1" t="s">
-        <v>281</v>
-      </c>
       <c r="E69" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F69" s="2"/>
+        <v>23</v>
+      </c>
+      <c r="F69" s="13">
+        <v>98.5</v>
+      </c>
       <c r="G69" s="2">
-        <v>6.9371728010743103E-3</v>
+        <v>7.7542711396397504E-3</v>
       </c>
       <c r="H69" s="1">
-        <v>1.34E-2</v>
-      </c>
-      <c r="I69" s="17"/>
+        <v>8.6E-3</v>
+      </c>
+      <c r="I69" s="11"/>
       <c r="J69" s="12">
-        <v>1334036499</v>
+        <v>393787075</v>
       </c>
       <c r="K69" s="12">
-        <v>1237756284</v>
+        <v>364983189</v>
       </c>
     </row>
     <row r="70" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" s="10" t="s">
+        <v>281</v>
+      </c>
+      <c r="B70" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="B70" s="3" t="s">
+      <c r="C70" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="C70" s="1" t="s">
+      <c r="D70" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="D70" s="1" t="s">
-        <v>285</v>
-      </c>
       <c r="E70" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F70" s="13">
-        <v>98.5</v>
+        <v>10</v>
+      </c>
+      <c r="F70" s="2">
+        <v>98.2</v>
       </c>
       <c r="G70" s="2">
-        <v>7.7542711396397504E-3</v>
+        <v>1.50968609448268E-2</v>
       </c>
       <c r="H70" s="1">
-        <v>8.6E-3</v>
+        <v>1.6799999999999999E-2</v>
       </c>
       <c r="I70" s="11"/>
       <c r="J70" s="12">
-        <v>393787075</v>
+        <v>573897449</v>
       </c>
       <c r="K70" s="12">
-        <v>364983189</v>
+        <v>530592961</v>
       </c>
     </row>
     <row r="71" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" s="10" t="s">
+        <v>285</v>
+      </c>
+      <c r="B71" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="B71" s="3" t="s">
+      <c r="C71" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="C71" s="1" t="s">
+      <c r="D71" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="D71" s="1" t="s">
-        <v>289</v>
-      </c>
       <c r="E71" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F71" s="2">
-        <v>98.2</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="F71" s="2"/>
       <c r="G71" s="2">
-        <v>1.50968609448268E-2</v>
-      </c>
-      <c r="H71" s="1">
-        <v>1.6799999999999999E-2</v>
-      </c>
-      <c r="I71" s="11"/>
+        <v>4.9426952737241202E-3</v>
+      </c>
+      <c r="I71" s="17"/>
       <c r="J71" s="12">
-        <v>573897449</v>
+        <v>438243172</v>
       </c>
       <c r="K71" s="12">
-        <v>530592961</v>
+        <v>404997282</v>
       </c>
     </row>
     <row r="72" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" s="10" t="s">
+        <v>289</v>
+      </c>
+      <c r="B72" s="3" t="s">
         <v>290</v>
       </c>
-      <c r="B72" s="3" t="s">
+      <c r="C72" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="C72" s="1" t="s">
+      <c r="D72" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="D72" s="1" t="s">
-        <v>293</v>
-      </c>
       <c r="E72" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F72" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="F72" s="13">
+        <v>98.9</v>
+      </c>
       <c r="G72" s="2">
-        <v>4.9426952737241202E-3</v>
-      </c>
-      <c r="I72" s="17"/>
+        <v>3.0342709749982599E-2</v>
+      </c>
+      <c r="H72" s="1">
+        <v>3.3099999999999997E-2</v>
+      </c>
+      <c r="I72" s="11"/>
       <c r="J72" s="12">
-        <v>438243172</v>
+        <v>529188541</v>
       </c>
       <c r="K72" s="12">
-        <v>404997282</v>
+        <v>487823627</v>
       </c>
     </row>
     <row r="73" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="B73" s="3" t="s">
         <v>294</v>
       </c>
-      <c r="B73" s="3" t="s">
+      <c r="C73" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="C73" s="1" t="s">
+      <c r="D73" s="1" t="s">
         <v>296</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>297</v>
       </c>
       <c r="E73" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F73" s="13">
-        <v>98.9</v>
-      </c>
+      <c r="F73" s="2"/>
       <c r="G73" s="2">
-        <v>3.0342709749982599E-2</v>
+        <v>8.2716200165949307E-3</v>
       </c>
       <c r="H73" s="1">
-        <v>3.3099999999999997E-2</v>
+        <v>1.1699999999999999E-2</v>
       </c>
       <c r="I73" s="11"/>
       <c r="J73" s="12">
-        <v>529188541</v>
+        <v>624926871</v>
       </c>
       <c r="K73" s="12">
-        <v>487823627</v>
+        <v>575521489</v>
       </c>
     </row>
     <row r="74" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" s="10" t="s">
+        <v>297</v>
+      </c>
+      <c r="B74" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="B74" s="3" t="s">
+      <c r="C74" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="C74" s="1" t="s">
+      <c r="D74" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="D74" s="1" t="s">
-        <v>301</v>
-      </c>
       <c r="E74" s="2" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="F74" s="2"/>
       <c r="G74" s="2">
-        <v>8.2716200165949307E-3</v>
-      </c>
-      <c r="H74" s="1">
-        <v>1.1699999999999999E-2</v>
+        <v>1.0413186028220301E-2</v>
       </c>
       <c r="I74" s="11"/>
       <c r="J74" s="12">
-        <v>624926871</v>
+        <v>383461667</v>
       </c>
       <c r="K74" s="12">
-        <v>575521489</v>
+        <v>352871537</v>
       </c>
     </row>
     <row r="75" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="10" t="s">
+        <v>301</v>
+      </c>
+      <c r="B75" s="3" t="s">
         <v>302</v>
       </c>
-      <c r="B75" s="3" t="s">
+      <c r="C75" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="C75" s="1" t="s">
+      <c r="D75" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="D75" s="1" t="s">
-        <v>305</v>
-      </c>
       <c r="E75" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F75" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="F75" s="2">
+        <v>99.2</v>
+      </c>
       <c r="G75" s="2">
-        <v>1.0413186028220301E-2</v>
+        <v>1.3046551466868001E-2</v>
+      </c>
+      <c r="H75" s="1">
+        <v>1.55E-2</v>
       </c>
       <c r="I75" s="11"/>
       <c r="J75" s="12">
-        <v>383461667</v>
+        <v>466916863</v>
       </c>
       <c r="K75" s="12">
-        <v>352871537</v>
+        <v>428608692</v>
       </c>
     </row>
     <row r="76" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="B76" s="3" t="s">
         <v>306</v>
       </c>
-      <c r="B76" s="3" t="s">
+      <c r="C76" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="C76" s="1" t="s">
+      <c r="D76" s="1" t="s">
         <v>308</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>309</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F76" s="2">
-        <v>99.2</v>
-      </c>
+      <c r="F76" s="2"/>
       <c r="G76" s="2">
-        <v>1.3046551466868001E-2</v>
+        <v>1.8491070824833099E-2</v>
       </c>
       <c r="H76" s="1">
-        <v>1.55E-2</v>
+        <v>2.2400000000000003E-2</v>
       </c>
       <c r="I76" s="11"/>
       <c r="J76" s="12">
-        <v>466916863</v>
+        <v>426225143</v>
       </c>
       <c r="K76" s="12">
-        <v>428608692</v>
+        <v>389312447</v>
       </c>
     </row>
     <row r="77" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" s="10" t="s">
+        <v>309</v>
+      </c>
+      <c r="B77" s="3" t="s">
         <v>310</v>
       </c>
-      <c r="B77" s="3" t="s">
+      <c r="C77" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="C77" s="1" t="s">
+      <c r="D77" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="D77" s="1" t="s">
-        <v>313</v>
-      </c>
       <c r="E77" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F77" s="2"/>
+        <v>28</v>
+      </c>
+      <c r="F77" s="13">
+        <v>98.6</v>
+      </c>
       <c r="G77" s="2">
-        <v>1.8491070824833099E-2</v>
+        <v>2.6246674465062E-2</v>
       </c>
       <c r="H77" s="1">
-        <v>2.2400000000000003E-2</v>
+        <v>2.8199999999999999E-2</v>
       </c>
       <c r="I77" s="11"/>
       <c r="J77" s="12">
-        <v>426225143</v>
+        <v>488454474</v>
       </c>
       <c r="K77" s="12">
-        <v>389312447</v>
+        <v>446015746</v>
       </c>
     </row>
     <row r="78" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A78" s="10" t="s">
+        <v>313</v>
+      </c>
+      <c r="B78" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="B78" s="3" t="s">
+      <c r="C78" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="C78" s="1" t="s">
+      <c r="D78" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="D78" s="1" t="s">
-        <v>317</v>
-      </c>
       <c r="E78" s="2" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="F78" s="13">
-        <v>98.6</v>
+        <v>98.9</v>
       </c>
       <c r="G78" s="2">
-        <v>2.6246674465062E-2</v>
+        <v>2.3285074666582299E-3</v>
       </c>
       <c r="H78" s="1">
-        <v>2.8199999999999999E-2</v>
+        <v>5.1000000000000004E-3</v>
       </c>
       <c r="I78" s="11"/>
       <c r="J78" s="12">
-        <v>488454474</v>
+        <v>437975811</v>
       </c>
       <c r="K78" s="12">
-        <v>446015746</v>
+        <v>399761949</v>
       </c>
     </row>
     <row r="79" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" s="10" t="s">
+        <v>317</v>
+      </c>
+      <c r="B79" s="3" t="s">
         <v>318</v>
       </c>
-      <c r="B79" s="3" t="s">
+      <c r="C79" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="C79" s="1" t="s">
+      <c r="D79" s="1" t="s">
         <v>320</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>321</v>
       </c>
       <c r="E79" s="2" t="s">
         <v>10</v>
@@ -4017,199 +4004,178 @@
         <v>98.9</v>
       </c>
       <c r="G79" s="2">
-        <v>2.3285074666582299E-3</v>
+        <v>2.14718905484611E-2</v>
       </c>
       <c r="H79" s="1">
-        <v>5.1000000000000004E-3</v>
+        <v>2.6800000000000001E-2</v>
       </c>
       <c r="I79" s="11"/>
       <c r="J79" s="12">
-        <v>437975811</v>
+        <v>860983966</v>
       </c>
       <c r="K79" s="12">
-        <v>399761949</v>
+        <v>784265446</v>
       </c>
     </row>
     <row r="80" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A80" s="10" t="s">
+        <v>321</v>
+      </c>
+      <c r="B80" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="B80" s="3" t="s">
+      <c r="C80" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="C80" s="1" t="s">
+      <c r="D80" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="D80" s="1" t="s">
-        <v>325</v>
-      </c>
       <c r="E80" s="2" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="F80" s="13">
-        <v>98.9</v>
+        <v>98.8</v>
       </c>
       <c r="G80" s="2">
-        <v>2.14718905484611E-2</v>
+        <v>8.1117160728049302E-3</v>
       </c>
       <c r="H80" s="1">
-        <v>2.6800000000000001E-2</v>
+        <v>9.1999999999999998E-3</v>
       </c>
       <c r="I80" s="11"/>
       <c r="J80" s="12">
-        <v>860983966</v>
+        <v>435105082</v>
       </c>
       <c r="K80" s="12">
-        <v>784265446</v>
+        <v>396065961</v>
       </c>
     </row>
     <row r="81" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A81" s="10" t="s">
+        <v>325</v>
+      </c>
+      <c r="B81" s="3" t="s">
         <v>326</v>
       </c>
-      <c r="B81" s="3" t="s">
+      <c r="C81" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="C81" s="1" t="s">
+      <c r="D81" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="D81" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="E81" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F81" s="13">
-        <v>98.8</v>
+      <c r="E81" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F81" s="1">
+        <v>99.1</v>
       </c>
       <c r="G81" s="2">
-        <v>8.1117160728049302E-3</v>
-      </c>
-      <c r="H81" s="1">
-        <v>9.1999999999999998E-3</v>
-      </c>
-      <c r="I81" s="11"/>
+        <v>1.53234739203283E-2</v>
+      </c>
+      <c r="I81" s="21"/>
       <c r="J81" s="12">
-        <v>435105082</v>
+        <v>465583481</v>
       </c>
       <c r="K81" s="12">
-        <v>396065961</v>
+        <v>421000426</v>
       </c>
     </row>
     <row r="82" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A82" s="10" t="s">
+        <v>329</v>
+      </c>
+      <c r="B82" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="B82" s="3" t="s">
+      <c r="C82" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="C82" s="1" t="s">
+      <c r="D82" s="1" t="s">
         <v>332</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>333</v>
       </c>
       <c r="E82" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F82" s="1">
-        <v>99.1</v>
+        <v>98.8</v>
       </c>
       <c r="G82" s="2">
-        <v>1.53234739203283E-2</v>
-      </c>
-      <c r="I82" s="21"/>
+        <v>2.9226579328700101E-2</v>
+      </c>
+      <c r="H82" s="1">
+        <v>3.6000000000000004E-2</v>
+      </c>
+      <c r="I82" s="22"/>
       <c r="J82" s="12">
-        <v>465583481</v>
+        <v>373059487</v>
       </c>
       <c r="K82" s="12">
-        <v>421000426</v>
+        <v>337172335</v>
       </c>
     </row>
     <row r="83" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A83" s="10" t="s">
+        <v>333</v>
+      </c>
+      <c r="B83" s="3" t="s">
         <v>334</v>
       </c>
-      <c r="B83" s="3" t="s">
+      <c r="C83" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="C83" s="1" t="s">
+      <c r="D83" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="D83" s="1" t="s">
+      <c r="E83" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="E83" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="F83" s="1">
-        <v>98.8</v>
+        <v>98.4</v>
       </c>
       <c r="G83" s="2">
-        <v>2.9226579328700101E-2</v>
+        <v>2.1994546737007601E-2</v>
       </c>
       <c r="H83" s="1">
-        <v>3.6000000000000004E-2</v>
-      </c>
-      <c r="I83" s="22"/>
+        <v>2.12E-2</v>
+      </c>
+      <c r="I83" s="14"/>
       <c r="J83" s="12">
-        <v>373059487</v>
+        <v>499372863</v>
       </c>
       <c r="K83" s="12">
-        <v>337172335</v>
-      </c>
-    </row>
-    <row r="84" spans="1:11" ht="17" x14ac:dyDescent="0.2">
-      <c r="A84" s="10" t="s">
-        <v>338</v>
-      </c>
-      <c r="B84" s="3" t="s">
-        <v>339</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="E84" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="F84" s="1">
-        <v>98.4</v>
-      </c>
-      <c r="G84" s="2">
-        <v>2.1994546737007601E-2</v>
-      </c>
-      <c r="H84" s="1">
-        <v>2.12E-2</v>
-      </c>
-      <c r="I84" s="14"/>
-      <c r="J84" s="12">
-        <v>499372863</v>
-      </c>
-      <c r="K84" s="12">
         <v>449465048</v>
       </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A84" s="2"/>
+      <c r="C84" s="2"/>
+      <c r="E84" s="2"/>
+      <c r="F84" s="2"/>
+      <c r="I84" s="2"/>
+      <c r="J84" s="12"/>
+      <c r="K84" s="12"/>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85" s="2"/>
       <c r="C85" s="2"/>
-      <c r="E85" s="2"/>
-      <c r="F85" s="2"/>
-      <c r="I85" s="2"/>
       <c r="J85" s="12"/>
       <c r="K85" s="12"/>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86" s="2"/>
       <c r="C86" s="2"/>
+      <c r="E86" s="2"/>
+      <c r="F86" s="2"/>
+      <c r="G86" s="2"/>
+      <c r="H86" s="2"/>
+      <c r="I86" s="2"/>
       <c r="J86" s="12"/>
       <c r="K86" s="12"/>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87" s="2"/>
       <c r="C87" s="2"/>
+      <c r="D87" s="2"/>
       <c r="E87" s="2"/>
       <c r="F87" s="2"/>
       <c r="G87" s="2"/>
@@ -4234,11 +4200,6 @@
       <c r="A89" s="2"/>
       <c r="C89" s="2"/>
       <c r="D89" s="2"/>
-      <c r="E89" s="2"/>
-      <c r="F89" s="2"/>
-      <c r="G89" s="2"/>
-      <c r="H89" s="2"/>
-      <c r="I89" s="2"/>
       <c r="J89" s="12"/>
       <c r="K89" s="12"/>
     </row>
@@ -4253,6 +4214,11 @@
       <c r="A91" s="2"/>
       <c r="C91" s="2"/>
       <c r="D91" s="2"/>
+      <c r="E91" s="2"/>
+      <c r="F91" s="2"/>
+      <c r="G91" s="2"/>
+      <c r="H91" s="2"/>
+      <c r="I91" s="2"/>
       <c r="J91" s="12"/>
       <c r="K91" s="12"/>
     </row>
@@ -4308,11 +4274,11 @@
       <c r="A96" s="2"/>
       <c r="C96" s="2"/>
       <c r="D96" s="2"/>
-      <c r="E96" s="2"/>
-      <c r="F96" s="2"/>
-      <c r="G96" s="2"/>
-      <c r="H96" s="2"/>
-      <c r="I96" s="2"/>
+      <c r="E96" s="3"/>
+      <c r="F96" s="3"/>
+      <c r="G96" s="3"/>
+      <c r="H96" s="3"/>
+      <c r="I96" s="3"/>
       <c r="J96" s="12"/>
       <c r="K96" s="12"/>
     </row>
@@ -4332,11 +4298,6 @@
       <c r="A98" s="2"/>
       <c r="C98" s="2"/>
       <c r="D98" s="2"/>
-      <c r="E98" s="3"/>
-      <c r="F98" s="3"/>
-      <c r="G98" s="3"/>
-      <c r="H98" s="3"/>
-      <c r="I98" s="3"/>
       <c r="J98" s="12"/>
       <c r="K98" s="12"/>
     </row>
@@ -4344,6 +4305,11 @@
       <c r="A99" s="2"/>
       <c r="C99" s="2"/>
       <c r="D99" s="2"/>
+      <c r="E99" s="2"/>
+      <c r="F99" s="2"/>
+      <c r="G99" s="2"/>
+      <c r="H99" s="2"/>
+      <c r="I99" s="2"/>
       <c r="J99" s="12"/>
       <c r="K99" s="12"/>
     </row>
@@ -4351,20 +4317,8 @@
       <c r="A100" s="2"/>
       <c r="C100" s="2"/>
       <c r="D100" s="2"/>
-      <c r="E100" s="2"/>
-      <c r="F100" s="2"/>
-      <c r="G100" s="2"/>
-      <c r="H100" s="2"/>
-      <c r="I100" s="2"/>
       <c r="J100" s="12"/>
       <c r="K100" s="12"/>
-    </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A101" s="2"/>
-      <c r="C101" s="2"/>
-      <c r="D101" s="2"/>
-      <c r="J101" s="12"/>
-      <c r="K101" s="12"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -4423,34 +4377,33 @@
     <hyperlink ref="A54" r:id="rId53" xr:uid="{C0A2C4DB-20EC-D948-8051-7AA52443D657}"/>
     <hyperlink ref="A55" r:id="rId54" xr:uid="{56CB8890-9109-EB44-854C-8AC8BA9DF14D}"/>
     <hyperlink ref="A56" r:id="rId55" xr:uid="{420F2CCF-E09D-5A4D-8F59-7970F3F9672D}"/>
-    <hyperlink ref="A57" r:id="rId56" xr:uid="{85EF404D-F703-AD46-B616-466C8B0C2743}"/>
-    <hyperlink ref="A58" r:id="rId57" xr:uid="{0A7A90F5-E9AA-1A42-8ACD-13EA03556B73}"/>
-    <hyperlink ref="A59" r:id="rId58" xr:uid="{81306969-FD36-D14A-A823-63141FE0CCB5}"/>
-    <hyperlink ref="A60" r:id="rId59" xr:uid="{6CEC0B5F-C420-0C45-AAC4-0EA26E272CA3}"/>
-    <hyperlink ref="A61" r:id="rId60" xr:uid="{1175D392-0EC8-1945-A36D-6912DF554D5A}"/>
-    <hyperlink ref="A62" r:id="rId61" xr:uid="{529001BC-F099-5943-B695-34F1EBC5D0D1}"/>
-    <hyperlink ref="A63" r:id="rId62" xr:uid="{06D177D7-0829-0442-BBB5-409530C6EC94}"/>
-    <hyperlink ref="A64" r:id="rId63" xr:uid="{2B886004-5A9E-0D47-A542-6C2F6C8295F2}"/>
-    <hyperlink ref="A65" r:id="rId64" xr:uid="{A262B8FC-C2CE-124F-BC22-BE0DAC9D8FA1}"/>
-    <hyperlink ref="A66" r:id="rId65" xr:uid="{156D0C29-4BB5-DB40-8DF8-04629536B243}"/>
-    <hyperlink ref="A67" r:id="rId66" xr:uid="{B1E4140F-3965-D949-B3B1-CC7C59507BCD}"/>
-    <hyperlink ref="A68" r:id="rId67" xr:uid="{D3580391-D796-9242-8957-C24716DC65B6}"/>
-    <hyperlink ref="A69" r:id="rId68" xr:uid="{6A5E0968-54B2-1647-8089-4B69676FEB95}"/>
-    <hyperlink ref="A70" r:id="rId69" xr:uid="{CDA7F8D0-5A81-8042-BE06-252C5B7654F8}"/>
-    <hyperlink ref="A71" r:id="rId70" xr:uid="{CF8D2CAA-F6CF-8340-AE12-E87DFC464A18}"/>
-    <hyperlink ref="A72" r:id="rId71" xr:uid="{778912A8-8239-3D4F-AA61-8E5BF1000E84}"/>
-    <hyperlink ref="A73" r:id="rId72" xr:uid="{CF753EF9-16B2-1F40-9228-3295D830BEB7}"/>
-    <hyperlink ref="A74" r:id="rId73" xr:uid="{8C3D51CE-43CD-5044-A5CE-F091557AFF9A}"/>
-    <hyperlink ref="A75" r:id="rId74" xr:uid="{A4971DC5-40A7-F944-944B-3AE2E5D2CE2A}"/>
-    <hyperlink ref="A76" r:id="rId75" xr:uid="{431A4313-1B8B-2743-8315-62F4D82B9135}"/>
-    <hyperlink ref="A77" r:id="rId76" xr:uid="{78C90727-AC8B-0745-9937-75B769C032E2}"/>
-    <hyperlink ref="A78" r:id="rId77" xr:uid="{2CB10D8B-F706-554D-8F7D-52989FED9BFC}"/>
-    <hyperlink ref="A79" r:id="rId78" xr:uid="{61449233-F37A-5149-B491-C2B69B4EB168}"/>
-    <hyperlink ref="A80" r:id="rId79" xr:uid="{F9B4DB32-D1DC-7F47-9EE5-60C5A75E57C8}"/>
-    <hyperlink ref="A81" r:id="rId80" xr:uid="{CC16428B-DD13-044E-BF4B-100EE7D6E645}"/>
-    <hyperlink ref="A82" r:id="rId81" xr:uid="{AB138BEB-C93B-474F-B96E-D0FE7B4DABE7}"/>
-    <hyperlink ref="A83" r:id="rId82" xr:uid="{A78A06AB-4D90-C74E-9E10-A2A4F9600D77}"/>
-    <hyperlink ref="A84" r:id="rId83" xr:uid="{7D1DA9DA-B1FB-B74A-B097-DF7097E17C69}"/>
+    <hyperlink ref="A57" r:id="rId56" xr:uid="{0A7A90F5-E9AA-1A42-8ACD-13EA03556B73}"/>
+    <hyperlink ref="A58" r:id="rId57" xr:uid="{81306969-FD36-D14A-A823-63141FE0CCB5}"/>
+    <hyperlink ref="A59" r:id="rId58" xr:uid="{6CEC0B5F-C420-0C45-AAC4-0EA26E272CA3}"/>
+    <hyperlink ref="A60" r:id="rId59" xr:uid="{1175D392-0EC8-1945-A36D-6912DF554D5A}"/>
+    <hyperlink ref="A61" r:id="rId60" xr:uid="{529001BC-F099-5943-B695-34F1EBC5D0D1}"/>
+    <hyperlink ref="A62" r:id="rId61" xr:uid="{06D177D7-0829-0442-BBB5-409530C6EC94}"/>
+    <hyperlink ref="A63" r:id="rId62" xr:uid="{2B886004-5A9E-0D47-A542-6C2F6C8295F2}"/>
+    <hyperlink ref="A64" r:id="rId63" xr:uid="{A262B8FC-C2CE-124F-BC22-BE0DAC9D8FA1}"/>
+    <hyperlink ref="A65" r:id="rId64" xr:uid="{156D0C29-4BB5-DB40-8DF8-04629536B243}"/>
+    <hyperlink ref="A66" r:id="rId65" xr:uid="{B1E4140F-3965-D949-B3B1-CC7C59507BCD}"/>
+    <hyperlink ref="A67" r:id="rId66" xr:uid="{D3580391-D796-9242-8957-C24716DC65B6}"/>
+    <hyperlink ref="A68" r:id="rId67" xr:uid="{6A5E0968-54B2-1647-8089-4B69676FEB95}"/>
+    <hyperlink ref="A69" r:id="rId68" xr:uid="{CDA7F8D0-5A81-8042-BE06-252C5B7654F8}"/>
+    <hyperlink ref="A70" r:id="rId69" xr:uid="{CF8D2CAA-F6CF-8340-AE12-E87DFC464A18}"/>
+    <hyperlink ref="A71" r:id="rId70" xr:uid="{778912A8-8239-3D4F-AA61-8E5BF1000E84}"/>
+    <hyperlink ref="A72" r:id="rId71" xr:uid="{CF753EF9-16B2-1F40-9228-3295D830BEB7}"/>
+    <hyperlink ref="A73" r:id="rId72" xr:uid="{8C3D51CE-43CD-5044-A5CE-F091557AFF9A}"/>
+    <hyperlink ref="A74" r:id="rId73" xr:uid="{A4971DC5-40A7-F944-944B-3AE2E5D2CE2A}"/>
+    <hyperlink ref="A75" r:id="rId74" xr:uid="{431A4313-1B8B-2743-8315-62F4D82B9135}"/>
+    <hyperlink ref="A76" r:id="rId75" xr:uid="{78C90727-AC8B-0745-9937-75B769C032E2}"/>
+    <hyperlink ref="A77" r:id="rId76" xr:uid="{2CB10D8B-F706-554D-8F7D-52989FED9BFC}"/>
+    <hyperlink ref="A78" r:id="rId77" xr:uid="{61449233-F37A-5149-B491-C2B69B4EB168}"/>
+    <hyperlink ref="A79" r:id="rId78" xr:uid="{F9B4DB32-D1DC-7F47-9EE5-60C5A75E57C8}"/>
+    <hyperlink ref="A80" r:id="rId79" xr:uid="{CC16428B-DD13-044E-BF4B-100EE7D6E645}"/>
+    <hyperlink ref="A81" r:id="rId80" xr:uid="{AB138BEB-C93B-474F-B96E-D0FE7B4DABE7}"/>
+    <hyperlink ref="A82" r:id="rId81" xr:uid="{A78A06AB-4D90-C74E-9E10-A2A4F9600D77}"/>
+    <hyperlink ref="A83" r:id="rId82" xr:uid="{7D1DA9DA-B1FB-B74A-B097-DF7097E17C69}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>